<commit_message>
added distance calculation with extra details
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/DistanceCalcSampleDataReverse.xlsx
+++ b/pyloghub/sample_data/DistanceCalcSampleDataReverse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\log-hub\log_hub\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE8725-C97D-4239-A034-81368613C548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD96EB1-85DE-4553-9726-29818D823F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{8BAF933F-BB86-4786-AA58-3BE0C97230E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BAF933F-BB86-4786-AA58-3BE0C97230E1}"/>
   </bookViews>
   <sheets>
     <sheet name="coordinates" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,20 +530,20 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -563,75 +563,75 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C2">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>36.671350199999999</v>
+        <v>36.729529499999998</v>
       </c>
       <c r="F2">
-        <v>-119.8155354</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-119.708861260756</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C3">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>38.473225900000003</v>
+        <v>38.5815719</v>
       </c>
       <c r="F3">
-        <v>-121.2980706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-121.49439959999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C4">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4">
-        <v>33.777465800000002</v>
+        <v>33.785389449999997</v>
       </c>
       <c r="F4">
-        <v>-118.18848699999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-118.158049315311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C5">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -640,38 +640,38 @@
         <v>37.804455699999998</v>
       </c>
       <c r="F5">
-        <v>-122.2713562</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-122.27135629999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C6">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>35.244231999999997</v>
+        <v>35.373871200000004</v>
       </c>
       <c r="F6">
-        <v>-118.97366551899999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-119.01946390000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C7">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -680,18 +680,18 @@
         <v>33.834751599999997</v>
       </c>
       <c r="F7">
-        <v>-117.91173190000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.911732</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C8">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -700,38 +700,38 @@
         <v>33.749495099999997</v>
       </c>
       <c r="F8">
-        <v>-117.8732212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.8732213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C9">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>33.721999099999998</v>
+        <v>33.953354599999997</v>
       </c>
       <c r="F9">
-        <v>-116.0372471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.3961623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C10">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -740,18 +740,18 @@
         <v>37.9577016</v>
       </c>
       <c r="F10">
-        <v>-121.2907795</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-121.29077959999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C11">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -760,18 +760,18 @@
         <v>32.6400541</v>
       </c>
       <c r="F11">
-        <v>-117.0841954</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.08419550000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C12">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -780,18 +780,18 @@
         <v>33.685696900000003</v>
       </c>
       <c r="F12">
-        <v>-117.82598179999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.8259819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C13">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -800,38 +800,38 @@
         <v>37.548269699999999</v>
       </c>
       <c r="F13">
-        <v>-121.9885718</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-121.9885719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C14">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14">
-        <v>34.825301899999999</v>
+        <v>34.108344899999999</v>
       </c>
       <c r="F14">
-        <v>-116.0833143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.28976520000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C15">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -840,18 +840,18 @@
         <v>37.639097200000002</v>
       </c>
       <c r="F15">
-        <v>-120.9968781</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-120.9968782</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C16">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -860,38 +860,38 @@
         <v>34.092233499999999</v>
       </c>
       <c r="F16">
-        <v>-117.4350479</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.43504799999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C17">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17">
-        <v>34.197504799999997</v>
+        <v>34.197630799999999</v>
       </c>
       <c r="F17">
-        <v>-119.1770515</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-119.18038180000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C18">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -900,18 +900,18 @@
         <v>33.937517</v>
       </c>
       <c r="F18">
-        <v>-117.23059430000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.2305944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C19">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
@@ -920,38 +920,38 @@
         <v>33.678333600000002</v>
       </c>
       <c r="F19">
-        <v>-118.0000165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-118.0000166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C20">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20">
-        <v>34.142345499999998</v>
+        <v>34.192912</v>
       </c>
       <c r="F20">
-        <v>-118.248367</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-118.24624861475399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C21">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -960,18 +960,18 @@
         <v>34.3916641</v>
       </c>
       <c r="F21">
-        <v>-118.54258590000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-118.542586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C22">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -980,18 +980,18 @@
         <v>33.195869600000002</v>
       </c>
       <c r="F22">
-        <v>-117.3794833</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.3794834</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C23">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -1000,18 +1000,18 @@
         <v>33.7746292</v>
       </c>
       <c r="F23">
-        <v>-117.94637160000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.9463717</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C24">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
@@ -1020,18 +1020,18 @@
         <v>34.103319200000001</v>
       </c>
       <c r="F24">
-        <v>-117.5751734</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-117.57517350000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25">
-        <v>37.7647993</v>
+        <v>37.779280800000002</v>
       </c>
       <c r="C25">
-        <v>-122.4629896</v>
+        <v>-122.41923629999999</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
@@ -1040,7 +1040,7 @@
         <v>38.440467499999997</v>
       </c>
       <c r="F25">
-        <v>-122.7144313</v>
+        <v>-122.7144314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed sample data for reverse mode in distance calculation
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/DistanceCalcSampleDataReverse.xlsx
+++ b/pyloghub/sample_data/DistanceCalcSampleDataReverse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD96EB1-85DE-4553-9726-29818D823F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578C857D-2775-4A08-BA2A-60495ADC1803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BAF933F-BB86-4786-AA58-3BE0C97230E1}"/>
   </bookViews>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>